<commit_message>
Update of documentation and pkgdown
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -282,12 +282,6 @@
     <t>[@throneberry_relation_1955; @maguire_speed_1962; @kendrick_photocontrol_1969; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
   </si>
   <si>
-    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
-It is estimated as follows: 
-$$S = \frac{N_{1}}{T_{1}} + \frac{N_{2}}{T_{2}} + \frac{N_{3}}{T_{3}} + \cdots + \frac{N_{n}}{T_{n}}$$
-Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).</t>
-  </si>
-  <si>
     <t>It is the average length of time required for maximum germination of a seed lot and is estimated according to the following formula.
 $$\overline{T} = \frac{\sum_{i=1}^{k}N_{i}T_{i}}{\sum_{i=1}^{k}N_{i}}$$
 Where, $T_{i}$ is the time from the start of the experiment to the $i$th observation, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.
@@ -370,11 +364,6 @@
   </si>
   <si>
     <t>Mean germination percentage per unit time $\overline{GP}$</t>
-  </si>
-  <si>
-    <t>It is estimated as follows: 
-$$S_{accumulated} = \frac{N_{1}}{T_{1}} + \frac{N_{1} + N_{2}}{T_{2}} + \frac{N_{1} + N_{2} + N_{3}}{T_{3}} + \cdots +\frac{N_{1} + N_{2} + \cdots + N_{n}}{T_{n}}$$
-Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).</t>
   </si>
   <si>
     <t>It is estimated as follows:
@@ -580,12 +569,23 @@
   <si>
     <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds:_1994;  @labouriau_uma_1983; @scott_review_1984]</t>
   </si>
+  <si>
+    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
+It is estimated as follows: 
+$$S = \frac{N_{1}}{T_{1}} + \frac{N_{2}}{T_{2}} + \frac{N_{3}}{T_{3}} + \cdots + \frac{N_{n}}{T_{n}}$$
+Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $\cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).</t>
+  </si>
+  <si>
+    <t>It is estimated as follows: 
+$$S_{accumulated} = \frac{N_{1}}{T_{1}} + \frac{N_{1} + N_{2}}{T_{2}} + \frac{N_{1} + N_{2} + N_{3}}{T_{3}} + \cdots +\frac{N_{1} + N_{2} + \cdots + N_{n}}{T_{n}}$$
+Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $\cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,7 +743,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,10 +775,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -810,7 +809,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -986,14 +984,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
@@ -1003,7 +1001,7 @@
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="60">
       <c r="A2" s="6" t="s">
         <v>74</v>
       </c>
@@ -1043,7 +1041,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="90">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
@@ -1063,7 +1061,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="6" t="s">
         <v>27</v>
       </c>
@@ -1083,7 +1081,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1103,7 +1101,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="105">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1141,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1163,7 +1161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="135">
       <c r="A9" s="6" t="s">
         <v>72</v>
       </c>
@@ -1171,7 +1169,7 @@
         <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>10</v>
@@ -1183,7 +1181,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="90">
       <c r="A10" s="6" t="s">
         <v>73</v>
       </c>
@@ -1203,9 +1201,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="90">
       <c r="A11" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>48</v>
@@ -1223,7 +1221,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="120">
       <c r="A12" s="6" t="s">
         <v>71</v>
       </c>
@@ -1231,19 +1229,19 @@
         <v>67</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="105">
       <c r="A13" s="6" t="s">
         <v>80</v>
       </c>
@@ -1251,19 +1249,19 @@
         <v>68</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45">
       <c r="A14" s="6" t="s">
         <v>77</v>
       </c>
@@ -1271,19 +1269,19 @@
         <v>69</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="75">
       <c r="A15" s="6" t="s">
         <v>78</v>
       </c>
@@ -1294,16 +1292,16 @@
         <v>76</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45">
       <c r="A16" s="6" t="s">
         <v>81</v>
       </c>
@@ -1311,19 +1309,19 @@
         <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="135">
       <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1331,19 +1329,19 @@
         <v>54</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="105">
       <c r="A18" s="6" t="s">
         <v>30</v>
       </c>
@@ -1351,19 +1349,19 @@
         <v>55</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45">
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
@@ -1371,55 +1369,55 @@
         <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>100</v>
-      </c>
       <c r="F19" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60">
       <c r="A20" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="60">
       <c r="A21" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="165">
       <c r="A22" s="8" t="s">
         <v>32</v>
       </c>
@@ -1427,17 +1425,17 @@
         <v>59</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45">
       <c r="A23" s="8" t="s">
         <v>33</v>
       </c>
@@ -1445,17 +1443,17 @@
         <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30">
       <c r="A24" s="8" t="s">
         <v>34</v>
       </c>
@@ -1463,17 +1461,17 @@
         <v>59</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="60">
       <c r="A25" s="8" t="s">
         <v>35</v>
       </c>
@@ -1481,17 +1479,17 @@
         <v>60</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="8" t="s">
         <v>36</v>
       </c>
@@ -1499,17 +1497,17 @@
         <v>61</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="75">
       <c r="A27" s="8" t="s">
         <v>37</v>
       </c>
@@ -1517,35 +1515,35 @@
         <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="135">
       <c r="A28" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -1553,16 +1551,16 @@
         <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="60">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1570,52 +1568,52 @@
         <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="90">
       <c r="A31" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="105">
+      <c r="A32" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1625,22 +1623,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30">
       <c r="A1" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>2</v>
@@ -1652,48 +1650,48 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>137</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45">
       <c r="A3" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>138</v>
-      </c>
       <c r="C3" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>140</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>10</v>
@@ -1702,12 +1700,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>10</v>
@@ -1716,12 +1714,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>10</v>
@@ -1730,12 +1728,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="30">
       <c r="A8" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>10</v>
@@ -1744,12 +1742,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="30">
       <c r="A9" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>10</v>
@@ -1758,12 +1756,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="30">
       <c r="A10" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>152</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>10</v>
@@ -1772,12 +1770,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>10</v>
@@ -1786,12 +1784,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -1800,12 +1798,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="120">
       <c r="A13" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>10</v>
@@ -1814,24 +1812,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="30">
       <c r="A14" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30">
       <c r="A15" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>10</v>
@@ -1840,12 +1838,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="30">
       <c r="A16" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -1857,12 +1855,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed reference in WGP
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -228,9 +228,6 @@
     <t>Standard error of germination rate ($s_{\overline{V}}$)</t>
   </si>
   <si>
-    <t>Coefficient of velocity/rate of germination or Kotowski's coefficient of velocity ($CVG$)</t>
-  </si>
-  <si>
     <t>Germination rate as the reciprocal of the median time ($v_{50}$)</t>
   </si>
   <si>
@@ -587,9 +584,6 @@
     <t>Weighted germination percentage ($WGP$)</t>
   </si>
   <si>
-    <t>[@reddy_effect_1978]</t>
-  </si>
-  <si>
     <t>WeightGermPercent</t>
   </si>
   <si>
@@ -599,6 +593,12 @@
   </si>
   <si>
     <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
+  </si>
+  <si>
+    <t>Coefficient of velocity of germination ($CVG$) or Coefficient of rate of germination ($CRG$) or Kotowski's coefficient of velocity</t>
+  </si>
+  <si>
+    <t>[@reddy_effect_1985; @reddy_effect_1978]</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F31" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>19</v>
@@ -1123,7 +1123,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>9</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>9</v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>10</v>
@@ -1203,7 +1203,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1228,7 +1228,7 @@
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>37</v>
@@ -1254,36 +1254,36 @@
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>168</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1294,16 +1294,16 @@
         <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1317,53 +1317,53 @@
         <v>62</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1374,16 +1374,16 @@
         <v>43</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1394,103 +1394,103 @@
         <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="F19" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>167</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>31</v>
@@ -1498,20 +1498,20 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1522,101 +1522,101 @@
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>31</v>
@@ -1624,40 +1624,40 @@
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1682,7 +1682,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
@@ -1696,23 +1696,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1720,10 +1720,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
@@ -1732,10 +1732,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>10</v>
@@ -1746,10 +1746,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
@@ -1760,10 +1760,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>10</v>
@@ -1774,10 +1774,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>10</v>
@@ -1788,10 +1788,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>10</v>
@@ -1802,10 +1802,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>10</v>
@@ -1816,10 +1816,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>10</v>
@@ -1830,10 +1830,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
@@ -1844,10 +1844,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>10</v>
@@ -1858,22 +1858,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>10</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>

</xml_diff>

<commit_message>
Attempt to fix vignette building error
1. \r\n -> \n
2. Removed non breaking space
3. % ot \%
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="171">
   <si>
     <t>function</t>
   </si>
@@ -39,9 +39,6 @@
     <t>GermPercent</t>
   </si>
   <si>
-    <t>Percentage (%)</t>
-  </si>
-  <si>
     <t>Germination capacity</t>
   </si>
   <si>
@@ -60,11 +57,6 @@
     <t>Peak period of germination or Modal time of germination</t>
   </si>
   <si>
-    <t>With argument method specified as `"farooq"`,  it is computed according to the formula by [@coolbear_effect_1984] as follows:
-$$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
-Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time  $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
-  </si>
-  <si>
     <t>[@farooq_thermal_2005]</t>
   </si>
   <si>
@@ -78,12 +70,6 @@
   </si>
   <si>
     <t>TimeSpreadGerm</t>
-  </si>
-  <si>
-    <t>It is the time to reach 50% of final/maximum germination.
-With argument method specified as `"coolbear"`,  it is computed according to the formula by [@coolbear_effect_1984] as follows:
-$$t_{50}=T_{i}+\frac{(\frac{N+1}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
-Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$  respectively, when $N_{i} &lt; \frac{N + 1}{2} &lt; N_{j}$.</t>
   </si>
   <si>
     <t>It is the time for first germination to occur (e.g. First day of germination)</t>
@@ -207,9 +193,6 @@
   </si>
   <si>
     <t>Variance of germination time ($s_{T}^{2}$)</t>
-  </si>
-  <si>
-    <t>Germination percentage or Germinability  ($GP$)</t>
   </si>
   <si>
     <t>It is computed as follows:
@@ -271,13 +254,7 @@
     <t>time^-2^</t>
   </si>
   <si>
-    <t>% day ^-1^</t>
-  </si>
-  <si>
     <t>[@bradbeer_seed_1988; @wardle_allelopathic_1991; @haugland_experiments_1996; @de_santana_alise_2004]</t>
-  </si>
-  <si>
-    <t>% time^-1^</t>
   </si>
   <si>
     <t>[@evetts_germination_1972]</t>
@@ -310,14 +287,6 @@
 Where, $N_{g}$ is the number of germinated seeds and $T_{n}$is the total number of intervals (e.g. days) required for final germination.</t>
   </si>
   <si>
-    <t>It is the progressive total of cumulative germination percentage recorded at specific intervals for a set period of time and is estimated in terms of cumulative germination percentage ($G_{i}$) as follows:
-$$\sum n = \sum_{i=1}^{t}G_{i}$$
-Where, $G_{i}$  is the  cumulative germination percentage in time interval $i$ and $t$ is the  total number of time intervals.
-It also estimated in terms of partial germination percentage as follows:
-$$\sum n = \sum_{i=1}^{t}g_{i}(t-j)$$
-Where, $g_{i}$ is the germination (not cumulative, but partial germination) in time interval $i$  ($i$ varying from $0$ to $t$) and $t$ is the total number of time  intervals and $j = i - 1$.</t>
-  </si>
-  <si>
     <t>[@khan_effect_1984]</t>
   </si>
   <si>
@@ -349,11 +318,6 @@
     <t>Synchrony of germination ($Z$ index)</t>
   </si>
   <si>
-    <t>It is estimated as follows:
-$$CV_{T} =  \sqrt{\frac{s_{T}^{2}}{\overline{T}}}$$
-Where, $s_{T}^{2}$ is the variance of germination time and $\overline{T}$ is the mean germination time.</t>
-  </si>
-  <si>
     <t>[@primack_longevity_1985; @ranal_how_2006]</t>
   </si>
   <si>
@@ -409,25 +373,10 @@
     <t>Shape and steepness ($b$)</t>
   </si>
   <si>
-    <t>Time required for 50% of viable seeds to germinate.</t>
-  </si>
-  <si>
     <t>It is the  time at germination onset and is computed by solving four-parameter hill function after setting y to 0 as follows:
 $$lag = b\sqrt{\frac{-y_{0}c^{b}}{a + y_{0}}}$$</t>
   </si>
   <si>
-    <t>The duration between the time at germination onset ($lag$) and that at 50% germination ($c$).</t>
-  </si>
-  <si>
-    <t>Time required for 50% of total seeds to germinate.</t>
-  </si>
-  <si>
-    <t>Time required for 50% of viable/germinated seeds to germinate</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>$t_{50_{total}}$</t>
   </si>
   <si>
@@ -438,12 +387,6 @@
   </si>
   <si>
     <t>$t_{x_{germinated}}$</t>
-  </si>
-  <si>
-    <t>Time required for $x$% of total seeds to germinate.</t>
-  </si>
-  <si>
-    <t>Time required for $x$% of viable/germinated seeds to germinate</t>
   </si>
   <si>
     <t>It is the  time interval between the percentages of viable seeds specified in the arguments `umin` and `umin` to germinate.</t>
@@ -478,9 +421,6 @@
     <t>[@heydecker_seed_1972; @bewley_seeds:_1994]</t>
   </si>
   <si>
-    <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds:_1994;  @labouriau_uma_1983; @scott_review_1984]</t>
-  </si>
-  <si>
     <t>CVGermTime</t>
   </si>
   <si>
@@ -546,13 +486,7 @@
 $GV$ value can be modified ($GV_{mod}$), to consider the entire duration from the beginning of the test instead of just from the onset of germination.</t>
   </si>
   <si>
-    <t>Germination value  ($GV$) (Czabator)</t>
-  </si>
-  <si>
     <t>Germination value ($GV$) (Diavanshir and Pourbiek)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak value($PV$)  (Czabator) or Emergence Energy ($EE$) </t>
   </si>
   <si>
     <t>Coefficient of variation of the germination time ($CV_{T}$)</t>
@@ -587,25 +521,94 @@
     <t>WeightGermPercent</t>
   </si>
   <si>
+    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
+  </si>
+  <si>
+    <t>Coefficient of velocity of germination ($CVG$) or Coefficient of rate of germination ($CRG$) or Kotowski's coefficient of velocity</t>
+  </si>
+  <si>
+    <t>[@reddy_effect_1985; @reddy_effect_1978]</t>
+  </si>
+  <si>
+    <t>Germination percentage or Germinability ($GP$)</t>
+  </si>
+  <si>
+    <t>Percentage (\%)</t>
+  </si>
+  <si>
+    <t>\% day ^-1^</t>
+  </si>
+  <si>
+    <t>\% time^-1^</t>
+  </si>
+  <si>
+    <t>\%</t>
+  </si>
+  <si>
+    <t>Time required for 50\% of viable seeds to germinate.</t>
+  </si>
+  <si>
+    <t>The duration between the time at germination onset ($lag$) and that at 50\% germination ($c$).</t>
+  </si>
+  <si>
+    <t>Time required for 50\% of viable/germinated seeds to germinate</t>
+  </si>
+  <si>
+    <t>Time required for 50\% of total seeds to germinate.</t>
+  </si>
+  <si>
+    <t>Time required for $x$\% of viable/germinated seeds to germinate</t>
+  </si>
+  <si>
+    <t>Time required for $x$\% of total seeds to germinate.</t>
+  </si>
+  <si>
+    <t>It is the time to reach 50\% of final/maximum germination.
+With argument method specified as `"coolbear"`, it is computed according to the formula by [@coolbear_effect_1984] as follows:
+$$t_{50}=T_{i}+\frac{(\frac{N+1}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
+Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N + 1}{2} &lt; N_{j}$.</t>
+  </si>
+  <si>
+    <t>With argument method specified as `"farooq"`, it is computed according to the formula by [@coolbear_effect_1984] as follows:
+$$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
+Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
+  </si>
+  <si>
+    <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds:_1994; @labouriau_uma_1983; @scott_review_1984]</t>
+  </si>
+  <si>
     <t>It is estimated as follows:
 $$WGP = \frac{\sum_{i=1}^{t}(t-i+1)N_{i}}{t \times N} \times 100$$
-Where, $N_{i}$  is the  number of seeds that germinated in the time interval $i$ (not cumulative, but partial count), $N$ is the total number of seeds tested and $t$ is the  total number of time intervals.</t>
-  </si>
-  <si>
-    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
-  </si>
-  <si>
-    <t>Coefficient of velocity of germination ($CVG$) or Coefficient of rate of germination ($CRG$) or Kotowski's coefficient of velocity</t>
-  </si>
-  <si>
-    <t>[@reddy_effect_1985; @reddy_effect_1978]</t>
+Where, $N_{i}$ is the number of seeds that germinated in the time interval $i$ (not cumulative, but partial count), $N$ is the total number of seeds tested and $t$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>It is the progressive total of cumulative germination percentage recorded at specific intervals for a set period of time and is estimated in terms of cumulative germination percentage ($G_{i}$) as follows:
+$$\sum n = \sum_{i=1}^{t}G_{i}$$
+Where, $G_{i}$ is the cumulative germination percentage in time interval $i$ and $t$ is the total number of time intervals.
+It also estimated in terms of partial germination percentage as follows:
+$$\sum n = \sum_{i=1}^{t}g_{i}(t-j)$$
+Where, $g_{i}$ is the germination (not cumulative, but partial germination) in time interval $i$ ($i$ varying from $0$ to $t$) and $t$ is the total number of time intervals and $j = i - 1$.</t>
+  </si>
+  <si>
+    <t>Peak value($PV$) (Czabator) or Emergence Energy ($EE$)</t>
+  </si>
+  <si>
+    <t>Germination value ($GV$) (Czabator)</t>
+  </si>
+  <si>
+    <t>It is estimated as follows:
+$$CV_{T} = \sqrt{\frac{s_{T}^{2}}{\overline{T}}}$$
+Where, $s_{T}^{2}$ is the variance of germination time and $\overline{T}$ is the mean germination time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +627,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -672,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -684,10 +694,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -706,6 +712,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,637 +1039,663 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>34</v>
+      <c r="F2" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>30</v>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>31</v>
+      <c r="F6" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>35</v>
+        <v>131</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>140</v>
+      <c r="F9" s="8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>36</v>
+        <v>56</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>38</v>
+      <c r="F10" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>37</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>38</v>
+      <c r="F11" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>74</v>
+        <v>122</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>72</v>
+        <v>22</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>55</v>
+        <v>149</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>136</v>
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>42</v>
+        <v>130</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>81</v>
+        <v>126</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>77</v>
+        <v>23</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>24</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>79</v>
+      <c r="D19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>169</v>
+      <c r="E20" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>144</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>46</v>
+        <v>79</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>47</v>
+        <v>145</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="10" t="s">
-        <v>81</v>
+        <v>167</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>31</v>
+        <v>132</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>47</v>
+        <v>133</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>48</v>
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>49</v>
+        <v>168</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>150</v>
+        <v>123</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>50</v>
+        <v>169</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>83</v>
+        <v>135</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>50</v>
+        <v>137</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>159</v>
+        <v>136</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>41</v>
+        <v>140</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="12"/>
+        <v>139</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>166</v>
+      </c>
       <c r="E30" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="8"/>
+        <v>170</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>166</v>
+      </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>31</v>
+        <v>86</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>52</v>
+        <v>88</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>51</v>
+        <v>89</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="8"/>
+        <v>91</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>166</v>
+      </c>
       <c r="E33" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1671,7 +1709,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,216 +1719,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="C3" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B8" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B10" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B11" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="C13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B14" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed details of t50 in Table 3
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -563,17 +563,6 @@
     <t>Time required for $x$\% of total seeds to germinate.</t>
   </si>
   <si>
-    <t>It is the time to reach 50\% of final/maximum germination.
-With argument method specified as `"coolbear"`, it is computed according to the formula by [@coolbear_effect_1984] as follows:
-$$t_{50}=T_{i}+\frac{(\frac{N+1}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
-Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N + 1}{2} &lt; N_{j}$.</t>
-  </si>
-  <si>
-    <t>With argument method specified as `"farooq"`, it is computed according to the formula by [@coolbear_effect_1984] as follows:
-$$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
-Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
-  </si>
-  <si>
     <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds:_1994; @labouriau_uma_1983; @scott_review_1984]</t>
   </si>
   <si>
@@ -602,6 +591,17 @@
     <t>It is estimated as follows:
 $$CV_{T} = \sqrt{\frac{s_{T}^{2}}{\overline{T}}}$$
 Where, $s_{T}^{2}$ is the variance of germination time and $\overline{T}$ is the mean germination time.</t>
+  </si>
+  <si>
+    <t>It is the time to reach 50\% of final/maximum germination.
+With argument `method` specified as `"coolbear"`, it is computed as follows:
+$$t_{50}=T_{i}+\frac{(\frac{N+1}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
+Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N + 1}{2} &lt; N_{j}$.</t>
+  </si>
+  <si>
+    <t>With argument `method` specified as `"farooq"`, it is computed as follows:
+$$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
+Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
   </si>
 </sst>
 </file>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1158,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>142</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1178,7 +1178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>143</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1295,7 +1295,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1426,10 +1426,10 @@
         <v>147</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>75</v>
@@ -1449,7 +1449,7 @@
         <v>76</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>75</v>
@@ -1469,7 +1469,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>75</v>
@@ -1486,10 +1486,10 @@
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>75</v>
@@ -1509,7 +1509,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>75</v>
@@ -1529,7 +1529,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>75</v>
@@ -1549,7 +1549,7 @@
         <v>82</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>75</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>46</v>
@@ -1569,7 +1569,7 @@
         <v>123</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>75</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>47</v>
@@ -1589,7 +1589,7 @@
         <v>135</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>75</v>
@@ -1609,7 +1609,7 @@
         <v>136</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>75</v>
@@ -1629,7 +1629,7 @@
         <v>139</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
@@ -1646,10 +1646,10 @@
         <v>121</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>86</v>
@@ -1689,7 +1689,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
-Fixed typo in formula for CUG in Table 3. -Added reference for Coefficient of variation of the germination time in Table 3.
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E045CD-FE9B-470D-9D5D-3442D996365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
   <si>
     <t>function</t>
   </si>
@@ -490,11 +491,6 @@
   </si>
   <si>
     <t>Coefficient of variation of the germination time ($CV_{T}$)</t>
-  </si>
-  <si>
-    <t>It is computed as follows:
-$$CV_{T} = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}(\overline{T}-T_{i})^{2}N_{i}}$$
-Where, $\overline{T}$ is the the mean germination time, $T_{i}$ is the time from the start of the experiment to the $i$th observation (day for the example); $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation), and $k$ is the last time of germination.</t>
   </si>
   <si>
     <t>Coefficient of uniformity of germination ($CUG$)</t>
@@ -603,11 +599,19 @@
 $$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
 Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
   </si>
+  <si>
+    <t>It is computed as follows:
+$$CUG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}(\overline{T}-T_{i})^{2}N_{i}}$$
+Where, $\overline{T}$ is the the mean germination time, $T_{i}$ is the time from the start of the experiment to the $i$th observation (day for the example); $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation), and $k$ is the last time of germination.</t>
+  </si>
+  <si>
+    <t>[@gomes_curso_1960; @ranal_how_2006]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -811,6 +815,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -846,6 +867,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1021,11 +1059,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1098,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1069,7 +1107,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1160,13 +1198,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1180,13 +1218,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1280,7 +1318,7 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>52</v>
@@ -1289,13 +1327,13 @@
         <v>64</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1369,13 +1407,13 @@
         <v>126</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1389,7 +1427,7 @@
         <v>127</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>75</v>
@@ -1420,27 +1458,27 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="C20" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>42</v>
@@ -1449,7 +1487,7 @@
         <v>76</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>75</v>
@@ -1469,7 +1507,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>75</v>
@@ -1480,16 +1518,16 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>75</v>
@@ -1509,7 +1547,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>75</v>
@@ -1529,7 +1567,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>75</v>
@@ -1549,7 +1587,7 @@
         <v>82</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>75</v>
@@ -1560,7 +1598,7 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>46</v>
@@ -1569,7 +1607,7 @@
         <v>123</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>75</v>
@@ -1580,7 +1618,7 @@
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>47</v>
@@ -1589,7 +1627,7 @@
         <v>135</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>75</v>
@@ -1609,27 +1647,27 @@
         <v>136</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
@@ -1646,16 +1684,16 @@
         <v>121</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1689,7 +1727,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>87</v>
@@ -1705,7 +1743,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1750,7 +1788,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1773,7 +1811,7 @@
         <v>105</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1801,7 +1839,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1815,7 +1853,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1829,7 +1867,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1843,7 +1881,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1857,7 +1895,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1937,7 +1975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated GP in Table 3
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E045CD-FE9B-470D-9D5D-3442D996365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CADA3A-39F7-4ABA-9979-778162403678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,9 +419,6 @@
     <t>Calculated by integration of the fitted curve and proper normalisation.</t>
   </si>
   <si>
-    <t>[@heydecker_seed_1972; @bewley_seeds:_1994]</t>
-  </si>
-  <si>
     <t>CVGermTime</t>
   </si>
   <si>
@@ -438,9 +435,6 @@
     <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
   <si>
-    <t>[@grose_laboratory_1958; @timson_new_1965; @brown_representing_1988; @baskin_seeds:_1998; @goodchild_method_1971]</t>
-  </si>
-  <si>
     <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
 It is estimated as follows: 
 $$S = \frac{N_{1}}{T_{1}} + \frac{N_{2}}{T_{2}} + \frac{N_{3}}{T_{3}} + \cdots + \frac{N_{n}}{T_{n}}$$
@@ -526,9 +520,6 @@
     <t>[@reddy_effect_1985; @reddy_effect_1978]</t>
   </si>
   <si>
-    <t>Germination percentage or Germinability ($GP$)</t>
-  </si>
-  <si>
     <t>Percentage (\%)</t>
   </si>
   <si>
@@ -557,9 +548,6 @@
   </si>
   <si>
     <t>Time required for $x$\% of total seeds to germinate.</t>
-  </si>
-  <si>
-    <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds:_1994; @labouriau_uma_1983; @scott_review_1984]</t>
   </si>
   <si>
     <t>It is estimated as follows:
@@ -606,6 +594,18 @@
   </si>
   <si>
     <t>[@gomes_curso_1960; @ranal_how_2006]</t>
+  </si>
+  <si>
+    <t>[@heydecker_seed_1972; @bewley_seeds_1994]</t>
+  </si>
+  <si>
+    <t>[@kotowski_temperature_1926, @nichols_two_1968; @bewley_seeds_1994; @labouriau_uma_1983; @scott_review_1984]</t>
+  </si>
+  <si>
+    <t>[@grose_laboratory_1958; @timson_new_1965; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
+  </si>
+  <si>
+    <t>Germination percentage or Final germination percentage or Germinability ($GP$)</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1107,7 +1107,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1173,7 +1173,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1198,13 +1198,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1218,13 +1218,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
@@ -1253,7 +1253,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1304,7 +1304,7 @@
         <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>70</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>52</v>
@@ -1327,13 +1327,13 @@
         <v>64</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1398,22 +1398,22 @@
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1424,10 +1424,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>75</v>
@@ -1458,27 +1458,27 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>42</v>
@@ -1487,7 +1487,7 @@
         <v>76</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>75</v>
@@ -1507,7 +1507,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>75</v>
@@ -1518,27 +1518,27 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>44</v>
@@ -1547,7 +1547,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>75</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>44</v>
@@ -1567,7 +1567,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>75</v>
@@ -1587,7 +1587,7 @@
         <v>82</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>75</v>
@@ -1598,36 +1598,36 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>75</v>
@@ -1638,62 +1638,62 @@
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>120</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>87</v>
@@ -1788,7 +1788,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1811,7 +1811,7 @@
         <v>105</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1839,7 +1839,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,7 +1853,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,7 +1867,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,7 +1881,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,7 +1895,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Updated documentation for GermSpeed
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CADA3A-39F7-4ABA-9979-778162403678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E2808-AD1E-4B6A-BB05-3C1CB7857537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,19 +435,6 @@
     <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
   <si>
-    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
-It is estimated as follows: 
-$$S = \frac{N_{1}}{T_{1}} + \frac{N_{2}}{T_{2}} + \frac{N_{3}}{T_{3}} + \cdots + \frac{N_{n}}{T_{n}}$$
-Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $\cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).
-Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
-  </si>
-  <si>
-    <t>It is estimated as follows: 
-$$S_{accumulated} = \frac{N_{1}}{T_{1}} + \frac{N_{1} + N_{2}}{T_{2}} + \frac{N_{1} + N_{2} + N_{3}}{T_{3}} + \cdots +\frac{N_{1} + N_{2} + \cdots + N_{n}}{T_{n}}$$
-Where, $N_{1}$, $N_{2}$, $N_{3}$, $\cdots$, $N_{n}$ are the number of germinated seeds observed at time (days or hours) $T_{1}$, $T_{2}$, $T_{3}$, $\cdots$, $T_{n}$ after sowing. (Not accumulated/cumulative number, but the number of seeds that germinated at the specific time).
-Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
-  </si>
-  <si>
     <t>[@al-mudaris_notes_1998; @schrader_seed_2000; @kader_comparison_2005]</t>
   </si>
   <si>
@@ -606,6 +593,22 @@
   </si>
   <si>
     <t>Germination percentage or Final germination percentage or Germinability ($GP$)</t>
+  </si>
+  <si>
+    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
+It is estimated as follows: 
+$$S = \sum_{i=1}^{k}\frac{N_{i}}{T_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the
+$i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.
+Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
+  </si>
+  <si>
+    <t>It is the rate of germination in terms of the accumulated/cumulative total number of seeds that germinate in a time interval.
+It is estimated as follows: 
+$$S_{accumulated} = \sum_{i=1}^{k}\frac{\sum_{j=1}^{i}N_{i}}{T_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the
+$i$th interval, $\sum_{j=1}^{i}N_{i}$ is the cumuative/accumulated number of seeds germinated in the $i$th interval and $k$ is the total number of time intervals.
+Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
   </si>
 </sst>
 </file>
@@ -1062,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1101,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1107,7 +1110,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1158,7 +1161,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1173,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1198,13 +1201,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1218,13 +1221,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1238,7 +1241,7 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
@@ -1318,7 +1321,7 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>52</v>
@@ -1327,13 +1330,13 @@
         <v>64</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1396,24 +1399,24 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
+        <v>170</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1424,10 +1427,10 @@
         <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>125</v>
+        <v>171</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>75</v>
@@ -1458,27 +1461,27 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>42</v>
@@ -1487,7 +1490,7 @@
         <v>76</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>75</v>
@@ -1507,7 +1510,7 @@
         <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>75</v>
@@ -1518,27 +1521,27 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>44</v>
@@ -1547,7 +1550,7 @@
         <v>83</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>75</v>
@@ -1558,7 +1561,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>44</v>
@@ -1567,7 +1570,7 @@
         <v>84</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>75</v>
@@ -1587,7 +1590,7 @@
         <v>82</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>75</v>
@@ -1598,7 +1601,7 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>46</v>
@@ -1607,27 +1610,27 @@
         <v>122</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>75</v>
@@ -1638,62 +1641,62 @@
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>75</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>120</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1727,7 +1730,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>87</v>
@@ -1788,7 +1791,7 @@
         <v>103</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1811,7 +1814,7 @@
         <v>105</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1839,7 +1842,7 @@
         <v>97</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,7 +1856,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,7 +1870,7 @@
         <v>109</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,7 +1884,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,7 +1898,7 @@
         <v>111</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Updated documentation for CUGerm
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50E2808-AD1E-4B6A-BB05-3C1CB7857537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E5551-63EC-40BE-B2D2-95E59EF39F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,11 +575,6 @@
 Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
   </si>
   <si>
-    <t>It is computed as follows:
-$$CUG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}(\overline{T}-T_{i})^{2}N_{i}}$$
-Where, $\overline{T}$ is the the mean germination time, $T_{i}$ is the time from the start of the experiment to the $i$th observation (day for the example); $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation), and $k$ is the last time of germination.</t>
-  </si>
-  <si>
     <t>[@gomes_curso_1960; @ranal_how_2006]</t>
   </si>
   <si>
@@ -609,6 +604,11 @@
 Where, $T_{i}$ is the time from the start of the experiment to the
 $i$th interval, $\sum_{j=1}^{i}N_{i}$ is the cumuative/accumulated number of seeds germinated in the $i$th interval and $k$ is the total number of time intervals.
 Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
+  </si>
+  <si>
+    <t>It is computed as follows:
+$$CUG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}(\overline{T}-T_{i})^{2}N_{i}}$$
+Where, $\overline{T}$ is the the mean germination time, $T_{i}$ is the time from the start of the experiment to the $i$th interval (day for the example); $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval), and $k$ is the total number of time intervals.</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1336,7 +1336,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1407,7 +1407,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>148</v>
@@ -1427,7 +1427,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>148</v>
@@ -1536,7 +1536,7 @@
         <v>75</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>157</v>
@@ -1676,7 +1676,7 @@
         <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
         <v>86</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated documentation for MeanGermRate 2
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3E5551-63EC-40BE-B2D2-95E59EF39F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23288CBD-CCD1-4816-AD8D-9FF2671431AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,11 +201,6 @@
 Where, $N_{g}$ is the number of germinated seeds and $N_{t}$ is the total number of seeds.</t>
   </si>
   <si>
-    <t>It is estimated according to the following formula.
-$$s_{\overline{V}} = \sqrt{\frac{s_{V}^{2}}{\sum_{i=1}^{k}N_{i}}}$$
-Where, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.</t>
-  </si>
-  <si>
     <t>Variance of germination rate ($s_{V}^{2}$)</t>
   </si>
   <si>
@@ -225,12 +220,6 @@
     <t>Standard error of germination time ($s_{\overline{T}}$)</t>
   </si>
   <si>
-    <t>It is estimated according to the following formula.
-$$CVG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}N_{i}T_{i}} \times 100$$
-$$CVG = \overline{V} \times 100$$
-Where, $T_{i}$ is the time from the start of the experiment to the $i$th observation, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.</t>
-  </si>
-  <si>
     <t>It is calculated according to the following formula.
 $$s_{V}^{2} = \overline{V}^{4} \times s_{T}^{2}$$
 Where, $s_{T}^{2}$ is the variance of germination time.</t>
@@ -420,13 +409,6 @@
   </si>
   <si>
     <t>CVGermTime</t>
-  </si>
-  <si>
-    <t>It is computed according to the following formula:
-$$\overline{V} = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}N_{i}T_{i}}$$
-Where, $T_{i}$ is the time from the start of the experiment to the $i$th observation, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.
-It is the inverse of mean germination time ($\overline{T}$).
-$$\overline{V} = \frac{1}{\overline{T}}$$</t>
   </si>
   <si>
     <t>It is the accumulated number of seeds germinated at the point on the germination curve at which the rate of germination starts to decrease. It is computed as the maximum quotient obtained by dividing successive cumulative germination values by the relevant incubation time.</t>
@@ -609,6 +591,24 @@
     <t>It is computed as follows:
 $$CUG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}(\overline{T}-T_{i})^{2}N_{i}}$$
 Where, $\overline{T}$ is the the mean germination time, $T_{i}$ is the time from the start of the experiment to the $i$th interval (day for the example); $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval), and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It is estimated according to the following formula.
+$$s_{\overline{V}} = \sqrt{\frac{s_{V}^{2}}{\sum_{i=1}^{k}N_{i}}}$$
+Where, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It is computed according to the following formula:
+$$\overline{V} = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}N_{i}T_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.
+It is the inverse of mean germination time ($\overline{T}$).
+$$\overline{V} = \frac{1}{\overline{T}}$$</t>
+  </si>
+  <si>
+    <t>It is estimated according to the following formula.
+$$CVG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}N_{i}T_{i}} \times 100$$
+$$CVG = \overline{V} \times 100$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1110,7 +1110,7 @@
         <v>57</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1176,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1201,13 +1201,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1256,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1281,7 +1281,7 @@
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>34</v>
@@ -1307,116 +1307,116 @@
         <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>121</v>
+        <v>170</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>169</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1427,16 +1427,16 @@
         <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1447,113 +1447,113 @@
         <v>41</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -1561,22 +1561,22 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1587,156 +1587,156 @@
         <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +1761,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
@@ -1775,23 +1775,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>103</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1811,10 +1811,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>9</v>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>9</v>
@@ -1937,22 +1937,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>

</xml_diff>

<commit_message>
Updated documentation for MeanGermTime 2
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23288CBD-CCD1-4816-AD8D-9FF2671431AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677300B2-5EA2-4581-9290-2AB1005565AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,17 +128,6 @@
     <t>[@labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
   <si>
-    <t>It signifies the accuracy of the calculation of the mean germination time.
-It is estimated according to the following formula:
-$$s_{\overline{T}} = \sqrt{\frac{s_{T}^{2}}{\sum_{i=1}^{k}N_{i}}}$$
-Where, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.</t>
-  </si>
-  <si>
-    <t>It is computed according to the following formula.
-$$s_{T}^{2} = \frac{\sum_{i=1}^{k}N_{i}(T_{i}-\overline{T})^{2}}{\sum_{i=1}^{k}N_{i}-1}$$
-Where, $T_{i}$ is the time from the start of the experiment to the $i$th observation, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.</t>
-  </si>
-  <si>
     <t>CUGerm</t>
   </si>
   <si>
@@ -208,13 +197,6 @@
   </si>
   <si>
     <t>Germination rate as the reciprocal of the median time ($v_{50}$)</t>
-  </si>
-  <si>
-    <t>It is the average length of time required for maximum germination of a seed lot and is estimated according to the following formula.
-$$\overline{T} = \frac{\sum_{i=1}^{k}N_{i}T_{i}}{\sum_{i=1}^{k}N_{i}}$$
-Where, $T_{i}$ is the time from the start of the experiment to the $i$th observation, $N_{i}$ is the number of seeds germinated in the $i$th time (not the accumulated number, but the number correspondent to the $i$th observation) and $k$ is the last time of germination.
-It is the inverse of mean germination rate ($\overline{V}$).
-$$\overline{T} = \frac{1}{\overline{V}}$$</t>
   </si>
   <si>
     <t>Standard error of germination time ($s_{\overline{T}}$)</t>
@@ -609,6 +591,24 @@
 $$CVG = \frac{\sum_{i=1}^{k}N_{i}}{\sum_{i=1}^{k}N_{i}T_{i}} \times 100$$
 $$CVG = \overline{V} \times 100$$
 Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It is the average length of time required for maximum germination of a seed lot and is estimated according to the following formula.
+$$\overline{T} = \frac{\sum_{i=1}^{k}N_{i}T_{i}}{\sum_{i=1}^{k}N_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.
+It is the inverse of mean germination rate ($\overline{V}$).
+$$\overline{T} = \frac{1}{\overline{V}}$$</t>
+  </si>
+  <si>
+    <t>It is computed according to the following formula.
+$$s_{T}^{2} = \frac{\sum_{i=1}^{k}N_{i}(T_{i}-\overline{T})^{2}}{\sum_{i=1}^{k}N_{i}-1}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It signifies the accuracy of the calculation of the mean germination time.
+It is estimated according to the following formula:
+$$s_{\overline{T}} = \sqrt{\frac{s_{T}^{2}}{\sum_{i=1}^{k}N_{i}}}$$
+Where, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,16 +1101,16 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1176,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1201,13 +1201,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1256,18 +1256,18 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>170</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
@@ -1301,122 +1301,122 @@
     </row>
     <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>141</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1424,19 +1424,19 @@
         <v>23</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1444,116 +1444,116 @@
         <v>24</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E22" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -1561,22 +1561,22 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1584,159 +1584,159 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +1761,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
@@ -1775,23 +1775,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1811,10 +1811,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>9</v>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>9</v>
@@ -1937,22 +1937,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>

</xml_diff>

<commit_message>
Updated documentation for GermSynchrony & GermUncertainty
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677300B2-5EA2-4581-9290-2AB1005565AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3336D-2511-464B-86D7-F9D2B33B0697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,20 +293,10 @@
     <t>[@primack_longevity_1985; @ranal_how_2006]</t>
   </si>
   <si>
-    <t>It is computed as follows:
-$$Z=\frac{\sum_{i=1}^{k}C_{N_{i},2}}{C_{\Sigma N_{i},2}}$$
-Where, $C_{N_{i},2}$ is the partial combination of the two germinated seeds from among $N_{i}$, the number of seeds germinated on the $i$th time (estimated as $C_{N_{i},2}=\frac{N{i}(N{i}-1)}{2}$) and $C_{\Sigma N_{i},2}$ is the partial combination of the two germinated seeds from among the total number of seeds germinated at the final count, assuming that all seeds that germinated did so simultaneously.</t>
-  </si>
-  <si>
     <t>[@shannon_mathematical_1948; @labouriau_germination_1976; @labouriau_uma_1983]</t>
   </si>
   <si>
     <t>bit</t>
-  </si>
-  <si>
-    <t>It is estimated as follows:
-$$\overline{E} = -\sum_{i=1}^{k}f_{i}\log_{2}f_{i}$$
-Where, $f_{i}$ is the relative frequency of germination ($f_{i}=\frac{N_{i}}{\sum_{i=1}^{k}N_{i}}$), $N_{i}$ is the number of seeds germinated on the $i$th time and $k$ is the last day of observation.</t>
   </si>
   <si>
     <t>Germination parameters</t>
@@ -609,6 +599,16 @@
 It is estimated according to the following formula:
 $$s_{\overline{T}} = \sqrt{\frac{s_{T}^{2}}{\sum_{i=1}^{k}N_{i}}}$$
 Where, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It is estimated as follows:
+$$\overline{E} = -\sum_{i=1}^{k}f_{i}\log_{2}f_{i}$$
+Where, $f_{i}$ is the relative frequency of germination ($f_{i}=\frac{N_{i}}{\sum_{i=1}^{k}N_{i}}$), $N_{i}$ is the number of seeds germinated on the $i$th time interval and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>It is computed as follows:
+$$Z=\frac{\sum_{i=1}^{k}C_{N_{i},2}}{C_{\Sigma N_{i},2}}$$
+Where, $C_{N_{i},2}$ is the partial combination of the two germinated seeds from among $N_{i}$, the number of seeds germinated on the $i$th time interval (estimated as $C_{N_{i},2}=\frac{N{i}(N{i}-1)}{2}$) and $C_{\Sigma N_{i},2}$ is the partial combination of the two germinated seeds from among the total number of seeds germinated at the final count, assuming that all seeds that germinated did so simultaneously.</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1110,7 +1110,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1176,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1201,13 +1201,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1221,13 +1221,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1256,7 +1256,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1267,7 +1267,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1287,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
@@ -1307,7 +1307,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>65</v>
@@ -1321,22 +1321,22 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1367,7 +1367,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>65</v>
@@ -1401,22 +1401,22 @@
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1427,10 +1427,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>70</v>
@@ -1461,27 +1461,27 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
@@ -1490,7 +1490,7 @@
         <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>70</v>
@@ -1510,7 +1510,7 @@
         <v>75</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>70</v>
@@ -1521,27 +1521,27 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
@@ -1550,7 +1550,7 @@
         <v>78</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>70</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>42</v>
@@ -1570,7 +1570,7 @@
         <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>70</v>
@@ -1590,7 +1590,7 @@
         <v>77</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>70</v>
@@ -1601,36 +1601,36 @@
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>70</v>
@@ -1641,62 +1641,62 @@
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>81</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1707,16 +1707,16 @@
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>82</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1727,10 +1727,10 @@
         <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>82</v>
@@ -1761,7 +1761,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
@@ -1775,23 +1775,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1799,10 +1799,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1811,10 +1811,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>9</v>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>9</v>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
@@ -1949,10 +1949,10 @@
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>

</xml_diff>

<commit_message>
Updated formulas for MeanGermPercent, MeanGermNumber and WeightGermPercent
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E3336D-2511-464B-86D7-F9D2B33B0697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,19 +231,9 @@
     <t>[@evetts_germination_1972]</t>
   </si>
   <si>
-    <t>It is computed as follows:
-$$S_{corrected} = \frac{S}{FGP}$$
-Where, $FGP$: the final germination percentage or germinability.</t>
-  </si>
-  <si>
     <t>Mixed</t>
   </si>
   <si>
-    <t>It is estimated as follows:
-$$\overline{G} = \frac{GP}{T_{n}}$$
-Where, $GP$ is the final germination percentage and $T_{n}$ is the total number of intervals(e.g. days) required for final germination.</t>
-  </si>
-  <si>
     <t>[@czabator_germination_1962]</t>
   </si>
   <si>
@@ -252,11 +241,6 @@
   </si>
   <si>
     <t>Number of seeds germinated per unit time $\overline{N}$</t>
-  </si>
-  <si>
-    <t>It is estimated as follows:
-$$\overline{N} = \frac{N_{g}}{T_{n}}$$
-Where, $N_{g}$ is the number of germinated seeds and $T_{n}$is the total number of intervals (e.g. days) required for final germination.</t>
   </si>
   <si>
     <t>[@khan_effect_1984]</t>
@@ -489,11 +473,6 @@
   </si>
   <si>
     <t>Time required for $x$\% of total seeds to germinate.</t>
-  </si>
-  <si>
-    <t>It is estimated as follows:
-$$WGP = \frac{\sum_{i=1}^{t}(t-i+1)N_{i}}{t \times N} \times 100$$
-Where, $N_{i}$ is the number of seeds that germinated in the time interval $i$ (not cumulative, but partial count), $N$ is the total number of seeds tested and $t$ is the total number of time intervals.</t>
   </si>
   <si>
     <t/>
@@ -610,11 +589,31 @@
 $$Z=\frac{\sum_{i=1}^{k}C_{N_{i},2}}{C_{\Sigma N_{i},2}}$$
 Where, $C_{N_{i},2}$ is the partial combination of the two germinated seeds from among $N_{i}$, the number of seeds germinated on the $i$th time interval (estimated as $C_{N_{i},2}=\frac{N{i}(N{i}-1)}{2}$) and $C_{\Sigma N_{i},2}$ is the partial combination of the two germinated seeds from among the total number of seeds germinated at the final count, assuming that all seeds that germinated did so simultaneously.</t>
   </si>
+  <si>
+    <t>It is computed as follows:
+$$S_{corrected} = \frac{S}{FGP}$$
+Where, $FGP$ is the final germination percentage or germinability.</t>
+  </si>
+  <si>
+    <t>It is estimated as follows:
+$$\overline{GP} = \frac{GP}{k}$$
+Where, $GP$ is the final germination percentage and $k$ is the total number of time intervals (e.g. days) required for final germination.</t>
+  </si>
+  <si>
+    <t>It is estimated as follows:
+$$\overline{N} = \frac{N_{g}}{k}$$
+Where, $N_{g}$ is the number of germinated seeds at the end of the germination test and $k$ is the total number of time intervals (e.g. days) required for final germination.</t>
+  </si>
+  <si>
+    <t>It is estimated as follows:
+$$WGP = \frac{\sum_{i=1}^{k}(k-i+1)N_{i}}{k \times N} \times 100$$
+Where, $N_{i}$ is the number of seeds that germinated in the time interval $i$ (not cumulative, but partial count), $N$ is the total number of seeds tested and $k$ is the total number of time intervals.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -818,23 +817,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -870,23 +852,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1062,11 +1027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1066,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1110,7 +1075,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1161,7 +1126,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1176,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1201,13 +1166,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1221,13 +1186,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1241,13 +1206,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1256,7 +1221,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1267,7 +1232,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1287,7 +1252,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
@@ -1307,7 +1272,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>65</v>
@@ -1321,22 +1286,22 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1367,7 +1332,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>65</v>
@@ -1401,22 +1366,22 @@
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1427,13 +1392,13 @@
         <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>67</v>
@@ -1447,13 +1412,13 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>168</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>68</v>
@@ -1461,99 +1426,99 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>28</v>
@@ -1561,22 +1526,22 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1587,156 +1552,156 @@
         <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1746,7 +1711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1761,7 +1726,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>2</v>
@@ -1775,23 +1740,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1799,10 +1764,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11" t="s">
@@ -1811,10 +1776,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1825,10 +1790,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>9</v>
@@ -1839,10 +1804,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1853,10 +1818,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1867,10 +1832,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1881,10 +1846,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1895,10 +1860,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1909,10 +1874,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
@@ -1923,10 +1888,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>9</v>
@@ -1937,22 +1902,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>111</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>9</v>
@@ -1963,10 +1928,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -1978,7 +1943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added formula for PV
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B8310-6049-4E3F-B51F-CCDD3FB21DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="173">
   <si>
     <t>function</t>
   </si>
@@ -367,9 +368,6 @@
     <t>CVGermTime</t>
   </si>
   <si>
-    <t>It is the accumulated number of seeds germinated at the point on the germination curve at which the rate of germination starts to decrease. It is computed as the maximum quotient obtained by dividing successive cumulative germination values by the relevant incubation time.</t>
-  </si>
-  <si>
     <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
   <si>
@@ -392,12 +390,6 @@
   </si>
   <si>
     <t>[@czabator_germination_1962; @bonner_ideal_1967]</t>
-  </si>
-  <si>
-    <t>It is computed as follows:
-$$GV = PV \times MDG$$
-Where, $PV$ is the peak value and $MDG$ is the mean daily germination percentage from the onset of germination.
-It can also be computed for other time intervals of successive germination counts, by replacing $MDG$ with the mean germination percentage per unit time ($\overline{GP}$).</t>
   </si>
   <si>
     <t>It is computed as follows:
@@ -609,11 +601,27 @@
 $$WGP = \frac{\sum_{i=1}^{k}(k-i+1)N_{i}}{k \times N} \times 100$$
 Where, $N_{i}$ is the number of seeds that germinated in the time interval $i$ (not cumulative, but partial count), $N$ is the total number of seeds tested and $k$ is the total number of time intervals.</t>
   </si>
+  <si>
+    <t>It is computed as follows:
+$$GV = PV \times MDG$$
+Where, $PV$ is the peak value and $MDG$ is the mean daily germination percentage from the onset of germination.
+It can also be computed for other time intervals of successive germination counts, by replacing $MDG$ with the mean germination percentage per unit time ($\overline{GP}$).
+$GV$ value can be modified ($GV_{mod}$), to consider the entire duration from the beginning of the test instead of just from the onset of germination.</t>
+  </si>
+  <si>
+    <t>It is the accumulated number of seeds germinated at the point on the germination curve at which the rate of germination starts to decrease. It is computed as the maximum quotient obtained by dividing successive cumulative germination values by the relevant incubation time.
+$$PV = \max\left ( \frac{G_{1}}{T_{1}},\frac{G_{2}}{T_{2}},\cdots \frac{G_{k}}{T_{k}} \right )$$
+Where, Where, $T_{i}$ is the time from the start of the experiment to the
+$i$th interval, $G_{i}$ is the cumulative germination percentage in the $i$th time interval and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>[@czabator_germination_1962; @brown_representing_1988]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -642,12 +650,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -688,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -724,6 +738,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,6 +834,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -852,6 +886,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1027,11 +1078,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1117,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1075,7 +1126,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1126,7 +1177,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1141,7 +1192,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1166,13 +1217,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1186,13 +1237,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1206,13 +1257,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1221,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1232,7 +1283,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1252,7 +1303,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
@@ -1272,7 +1323,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>65</v>
@@ -1286,22 +1337,22 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1332,7 +1383,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>65</v>
@@ -1366,22 +1417,22 @@
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1392,10 +1443,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>69</v>
@@ -1412,7 +1463,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>65</v>
@@ -1426,36 +1477,36 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>145</v>
+        <v>169</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>69</v>
@@ -1472,10 +1523,10 @@
         <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>69</v>
@@ -1486,27 +1537,27 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
@@ -1515,7 +1566,7 @@
         <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>69</v>
@@ -1526,7 +1577,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>42</v>
@@ -1535,7 +1586,7 @@
         <v>76</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>69</v>
@@ -1555,7 +1606,7 @@
         <v>74</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>69</v>
@@ -1564,104 +1615,104 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>145</v>
+        <v>171</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>145</v>
+        <v>170</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>70</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>145</v>
+        <v>119</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1672,7 +1723,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>84</v>
@@ -1692,10 +1743,10 @@
         <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>79</v>
@@ -1711,7 +1762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1756,7 +1807,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1779,7 +1830,7 @@
         <v>95</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1807,7 +1858,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1821,7 +1872,7 @@
         <v>98</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1835,7 +1886,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1849,7 +1900,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1863,7 +1914,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>
@@ -1943,7 +1994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added references and updated documentation
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B8310-6049-4E3F-B51F-CCDD3FB21DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D26683-C857-4C59-95A9-72DB10F92FD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -368,19 +368,10 @@
     <t>CVGermTime</t>
   </si>
   <si>
-    <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
-  </si>
-  <si>
     <t>[@al-mudaris_notes_1998; @schrader_seed_2000; @kader_comparison_2005]</t>
   </si>
   <si>
     <t>Time spread of germination or Germination distribution</t>
-  </si>
-  <si>
-    <t>Speed of germination or Germination rate Index or index of velocity of germination or Emergence rate index (Germination index according to AOSA)</t>
-  </si>
-  <si>
-    <t>Mean germination time or Mean length of incubation time ($\overline{T}$) or Germination resistance ($GR$) or Sprouting index ($SI$)</t>
   </si>
   <si>
     <t>Modified Timson's index (Labouriau)</t>
@@ -426,9 +417,6 @@
   </si>
   <si>
     <t>WeightGermPercent</t>
-  </si>
-  <si>
-    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
   </si>
   <si>
     <t>Coefficient of velocity of germination ($CVG$) or Coefficient of rate of germination ($CRG$) or Kotowski's coefficient of velocity</t>
@@ -616,6 +604,18 @@
   </si>
   <si>
     <t>[@czabator_germination_1962; @brown_representing_1988]</t>
+  </si>
+  <si>
+    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbachTillageContinuousCorn1982; @aosa_seed_1983; @khandakar_jute_1983; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
+  </si>
+  <si>
+    <t>Speed of germination or Germination rate Index or index of velocity of germination or Emergence rate index (Allan, Vogel and Peterson; Erbach) or Germination index (AOSA)</t>
+  </si>
+  <si>
+    <t>Mean germination time or Mean length of incubation time ($\overline{T}$) or Germination resistance ($GR$) or Sprouting index ($SI$) or Emergence index ($EI$)</t>
+  </si>
+  <si>
+    <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @mockColdToleranceAdapted1972; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
 </sst>
 </file>
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
@@ -1126,7 +1126,7 @@
         <v>55</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
@@ -1192,7 +1192,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1217,13 +1217,13 @@
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>9</v>
@@ -1237,13 +1237,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -1257,13 +1257,13 @@
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>9</v>
@@ -1272,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1283,7 +1283,7 @@
         <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
@@ -1303,7 +1303,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>9</v>
@@ -1323,7 +1323,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>65</v>
@@ -1337,22 +1337,22 @@
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>65</v>
@@ -1417,22 +1417,22 @@
     </row>
     <row r="17" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1443,10 +1443,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>69</v>
@@ -1463,7 +1463,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>65</v>
@@ -1477,36 +1477,36 @@
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>69</v>
@@ -1523,10 +1523,10 @@
         <v>41</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>69</v>
@@ -1537,27 +1537,27 @@
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>42</v>
@@ -1566,7 +1566,7 @@
         <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>69</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>42</v>
@@ -1586,7 +1586,7 @@
         <v>76</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>69</v>
@@ -1606,7 +1606,7 @@
         <v>74</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>69</v>
@@ -1617,102 +1617,102 @@
     </row>
     <row r="27" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>84</v>
@@ -1743,10 +1743,10 @@
         <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>79</v>
@@ -1807,7 +1807,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -1830,7 +1830,7 @@
         <v>95</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>9</v>
@@ -1858,7 +1858,7 @@
         <v>87</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>9</v>
@@ -1872,7 +1872,7 @@
         <v>98</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>9</v>
@@ -1886,7 +1886,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>9</v>
@@ -1900,7 +1900,7 @@
         <v>100</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>9</v>
@@ -1914,7 +1914,7 @@
         <v>101</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Update references + bibtex key
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AF1F68-5DBB-4513-8F7E-146D15344692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,9 +437,6 @@
     <t>Mean germination time or Mean length of incubation time ($\overline{T}$) or Germination resistance ($GR$) or Sprouting index ($SI$) or Emergence index ($EI$)</t>
   </si>
   <si>
-    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbachTillageContinuousCorn1982; @aosa_seed_1983; @khandakar_jute_1983; @hsuPlantingDateEffects1986; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
-  </si>
-  <si>
     <t>Speed of germination or Germination rate Index or index of velocity of germination or Emergence rate index (Allan, Vogel and Peterson; Erbach; Hsu and Nelson) or Germination index (AOSA)</t>
   </si>
   <si>
@@ -451,9 +449,6 @@
   <si>
     <t>It is estimated as Timson's index ($\Sigma k$) divided by the total time period of germination ($T_{k}$).
 $$\Sigma k_{mod} = \frac{\Sigma k}{T_{k}}$$</t>
-  </si>
-  <si>
-    <t>[@grose_laboratory_1958; @timson_new_1965; @lyonRapidMethodDetermining1966; @chaudharyEffectTemperatureAssociated1970; @negmEffectsEthyleneCarbon1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
   </si>
   <si>
     <t>Germination unifromity</t>
@@ -691,11 +686,17 @@
 It is the inverse of mean germination rate ($\overline{V}$).
 $$\overline{T} = \frac{1}{\overline{V}}$$</t>
   </si>
+  <si>
+    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbachTillageContinuousCorn1982; @aosa_seed_1983; @khandakar_jute_1983; @hsu_planting_1986; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
+  </si>
+  <si>
+    <t>[@grose_laboratory_1958; @timson_new_1965; @lyonRapidMethodDetermining1966; @chaudharyEffectTemperatureAssociated1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,6 +905,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -939,6 +957,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1114,11 +1149,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1159,7 +1194,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>116</v>
@@ -1259,7 +1294,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>8</v>
@@ -1279,7 +1314,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>8</v>
@@ -1299,7 +1334,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
@@ -1308,7 +1343,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1319,7 +1354,7 @@
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1359,7 +1394,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>62</v>
@@ -1379,7 +1414,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>117</v>
@@ -1419,7 +1454,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>62</v>
@@ -1453,13 +1488,13 @@
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>118</v>
@@ -1468,7 +1503,7 @@
         <v>66</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>136</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1479,7 +1514,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>118</v>
@@ -1499,7 +1534,7 @@
         <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>62</v>
@@ -1519,7 +1554,7 @@
         <v>113</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>126</v>
@@ -1539,7 +1574,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>126</v>
@@ -1559,7 +1594,7 @@
         <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>126</v>
@@ -1579,7 +1614,7 @@
         <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>126</v>
@@ -1588,18 +1623,18 @@
         <v>66</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>126</v>
@@ -1613,13 +1648,13 @@
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>126</v>
@@ -1633,13 +1668,13 @@
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>126</v>
@@ -1653,110 +1688,110 @@
     </row>
     <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="8" t="s">
         <v>66</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1767,7 +1802,7 @@
         <v>42</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>118</v>
@@ -1787,7 +1822,7 @@
         <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>126</v>
@@ -1807,7 +1842,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>126</v>
@@ -1827,13 +1862,13 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>126</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>130</v>
@@ -1847,13 +1882,13 @@
         <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>126</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>129</v>
@@ -1867,7 +1902,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>77</v>
@@ -1887,7 +1922,7 @@
         <v>44</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>126</v>
@@ -1906,7 +1941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -1988,7 +2023,7 @@
         <v>79</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>8</v>
@@ -2086,7 +2121,7 @@
         <v>95</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>8</v>
@@ -2126,7 +2161,7 @@
         <v>82</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2138,7 +2173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Add equations to t0, tg and tpeak
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AF1F68-5DBB-4513-8F7E-146D15344692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933793EA-08EC-4C05-83DA-199DFAFA2D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,9 +55,6 @@
     <t>[@coolbear_effect_1984]</t>
   </si>
   <si>
-    <t>Peak period of germination or Modal time of germination</t>
-  </si>
-  <si>
     <t>[@farooq_thermal_2005]</t>
   </si>
   <si>
@@ -73,12 +70,6 @@
     <t>TimeSpreadGerm</t>
   </si>
   <si>
-    <t>It is the time for first germination to occur (e.g. First day of germination)</t>
-  </si>
-  <si>
-    <t>It is the time for last germination to occur (e.g. Last day of germination)</t>
-  </si>
-  <si>
     <t>Time for the first germination or Germination time lag ($t_{0}$)</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
   </si>
   <si>
     <t>Corrected germination rate index</t>
-  </si>
-  <si>
-    <t>It is the time in which highest frequency of germinated seeds are observed and need not be unique.</t>
   </si>
   <si>
     <t>[@edwards_temperature_1932]</t>
@@ -691,6 +679,24 @@
   </si>
   <si>
     <t>[@grose_laboratory_1958; @timson_new_1965; @lyonRapidMethodDetermining1966; @chaudharyEffectTemperatureAssociated1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
+  </si>
+  <si>
+    <t>It is the time for last germination to occur (e.g. Last day of germination)
+$$t_{g} = \max \left\{ T_{i} : N_{i} \neq  0 \right\}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval and $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval)</t>
+  </si>
+  <si>
+    <t>It is the time for first germination to occur (e.g. First day of germination).
+$$t_{0} = \min \left\{ T_{i} : N_{i} \neq  0 \right\}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval and $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval)</t>
+  </si>
+  <si>
+    <t>It is the time in which highest frequency of germinated seeds are observed and need not be unique.
+$$t_{peak} = \left\{ T_{i} : N_{i} = N_{max} \right\}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval) and $N_{max}$ is the maximum number of seeds germinated per interval.</t>
+  </si>
+  <si>
+    <t>Peak period of germination or Modal time of germination ($t_{peak}$)</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1188,33 +1194,33 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>17</v>
+        <v>190</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>8</v>
@@ -1223,18 +1229,18 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>18</v>
+        <v>189</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1243,18 +1249,18 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -1263,18 +1269,18 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>24</v>
+        <v>191</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
@@ -1283,18 +1289,18 @@
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>8</v>
@@ -1308,13 +1314,13 @@
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>8</v>
@@ -1323,18 +1329,18 @@
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
@@ -1343,18 +1349,18 @@
         <v>9</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1363,18 +1369,18 @@
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>8</v>
@@ -1383,555 +1389,555 @@
         <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="D14" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>66</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D36" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>77</v>
-      </c>
       <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1956,7 +1962,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>1</v>
@@ -1970,23 +1976,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>6</v>
@@ -1994,22 +2000,22 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>8</v>
@@ -2020,10 +2026,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>8</v>
@@ -2034,10 +2040,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>8</v>
@@ -2048,10 +2054,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>8</v>
@@ -2062,10 +2068,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>8</v>
@@ -2076,10 +2082,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>8</v>
@@ -2090,10 +2096,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -2104,10 +2110,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>8</v>
@@ -2118,10 +2124,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>8</v>
@@ -2132,22 +2138,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>8</v>
@@ -2158,10 +2164,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>

</xml_diff>

<commit_message>
Update and fix units
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6C6350-B731-4D01-B4E0-5A5013904980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200D58D-259B-41E5-93E1-4C1259BFC8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="204">
   <si>
     <t>Germination index</t>
   </si>
@@ -363,9 +363,6 @@
   </si>
   <si>
     <t>Percentage (\%)</t>
-  </si>
-  <si>
-    <t>\% day ^-1^</t>
   </si>
   <si>
     <t>\% time^-1^</t>
@@ -504,12 +501,6 @@
     <t>EmergenceRateIndex</t>
   </si>
   <si>
-    <t>It is the accumulated number of seeds germinated at the point on the germination curve at which the rate of germination starts to decrease. It is computed as the maximum quotient obtained by dividing successive cumulative germination values by the relevant incubation time.
-$$PV = \max\left ( \frac{G_{1}}{T_{1}},\frac{G_{2}}{T_{2}},\cdots \frac{G_{k}}{T_{k}} \right )$$
-Where, $T_{i}$ is the time from the start of the experiment to the
-$i$th interval, $G_{i}$ is the cumulative germination percentage in the $i$th time interval, and $k$ is the total number of time intervals.</t>
-  </si>
-  <si>
     <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @mockColdToleranceAdapted1972; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
   </si>
   <si>
@@ -569,22 +560,6 @@
     <t>With argument `method` specified as `"farooq"`, it is computed as follows.
 $$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
 Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds, and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
-  </si>
-  <si>
-    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
-It is estimated as follows.
-$$S = \sum_{i=1}^{k}\frac{N_{i}}{T_{i}}$$
-Where, $T_{i}$ is the time from the start of the experiment to the
-$i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval), and $k$ is the total number of time intervals.
-Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
-  </si>
-  <si>
-    <t>It is the rate of germination in terms of the accumulated/cumulative total number of seeds that germinate in a time interval.
-It is estimated as follows.
-$$S_{accumulated} = \sum_{i=1}^{k}\frac{\sum_{j=1}^{i}N_{j}}{T_{i}}$$
-Where, $T_{i}$ is the time from the start of the experiment to the
-$i$th interval, $\sum_{j=1}^{i}N_{j}$ is the cumuative/accumulated number of seeds germinated in the $i$th interval, and $k$ is the total number of time intervals.
-Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
   </si>
   <si>
     <t>It is computed as follows.
@@ -711,6 +686,49 @@
   </si>
   <si>
     <t>[@vallance_studies_1950; @roh_maturity_2004]</t>
+  </si>
+  <si>
+    <t>no unit</t>
+  </si>
+  <si>
+    <t>It is the rate of germination in terms of the total number of seeds that germinate in a time interval. 
+It is estimated as follows.
+$$S = \sum_{i=1}^{k}\frac{N_{i}}{T_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $N_{i}$ is the number of seeds germinated in the $i$th time interval (not the accumulated number, but the number corresponding to the $i$th interval), and $k$ is the total number of time intervals.
+Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
+  </si>
+  <si>
+    <t>It is the rate of germination in terms of the accumulated/cumulative total number of seeds that germinate in a time interval.
+It is estimated as follows.
+$$S_{accumulated} = \sum_{i=1}^{k}\frac{\sum_{j=1}^{i}N_{j}}{T_{i}}$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $\sum_{j=1}^{i}N_{j}$ is the cumuative/accumulated number of seeds germinated in the $i$th interval, and $k$ is the total number of time intervals.
+Instead of germination counts, germination percentages may also be used for computation of speed of germination.</t>
+  </si>
+  <si>
+    <t>It is the accumulated number of seeds germinated at the point on the germination curve at which the rate of germination starts to decrease. It is computed as the maximum quotient obtained by dividing successive cumulative germination values by the relevant incubation time.
+$$PV = \max\left ( \frac{G_{1}}{T_{1}},\frac{G_{2}}{T_{2}},\cdots \frac{G_{k}}{T_{k}} \right )$$
+Where, $T_{i}$ is the time from the start of the experiment to the $i$th interval, $G_{i}$ is the cumulative germination percentage in the $i$th time interval, and $k$ is the total number of time intervals.</t>
+  </si>
+  <si>
+    <t>count time^-1^</t>
+  </si>
+  <si>
+    <t>\% time^-1^ or count time^-1^</t>
+  </si>
+  <si>
+    <t>count time</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>time count^-1^</t>
+  </si>
+  <si>
+    <t>\%^2^ time^-2^</t>
+  </si>
+  <si>
+    <t>\%^2^ time^-1^</t>
   </si>
 </sst>
 </file>
@@ -739,18 +757,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -822,9 +834,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -832,6 +841,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,7 +1185,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1208,13 +1220,13 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>112</v>
@@ -1228,13 +1240,13 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>112</v>
@@ -1243,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1254,7 +1266,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1274,7 +1286,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -1308,13 +1320,13 @@
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>8</v>
@@ -1334,7 +1346,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>8</v>
@@ -1354,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
@@ -1368,13 +1380,13 @@
     </row>
     <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1383,7 +1395,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1394,10 +1406,10 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -1414,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>8</v>
@@ -1434,7 +1446,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>58</v>
@@ -1454,7 +1466,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>113</v>
@@ -1463,7 +1475,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1494,7 +1506,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>58</v>
@@ -1528,22 +1540,22 @@
     </row>
     <row r="18" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>114</v>
+        <v>194</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1554,10 +1566,10 @@
         <v>32</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>114</v>
+        <v>195</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>62</v>
@@ -1574,7 +1586,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>58</v>
@@ -1594,10 +1606,10 @@
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>122</v>
+        <v>169</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>112</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>62</v>
@@ -1614,10 +1626,10 @@
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>62</v>
@@ -1634,10 +1646,10 @@
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>122</v>
+        <v>197</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>62</v>
@@ -1654,30 +1666,30 @@
         <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>62</v>
@@ -1688,16 +1700,16 @@
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>62</v>
@@ -1708,16 +1720,16 @@
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>62</v>
@@ -1728,124 +1740,136 @@
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="6"/>
+        <v>160</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="E28" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="6"/>
+        <v>159</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="E29" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>200</v>
+      </c>
       <c r="E30" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" s="6"/>
+        <v>163</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>193</v>
+      </c>
       <c r="E31" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D32" s="6"/>
+        <v>161</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>197</v>
+      </c>
       <c r="E32" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D33" s="6"/>
+        <v>154</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>201</v>
+      </c>
       <c r="E33" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>62</v>
@@ -1856,22 +1880,22 @@
     </row>
     <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>122</v>
+        <v>173</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="165" x14ac:dyDescent="0.25">
@@ -1882,10 +1906,10 @@
         <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>122</v>
+        <v>174</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>62</v>
@@ -1902,16 +1926,16 @@
         <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1922,16 +1946,16 @@
         <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1942,7 +1966,7 @@
         <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>73</v>
@@ -1962,10 +1986,10 @@
         <v>40</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>122</v>
+        <v>193</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>68</v>
@@ -1995,216 +2019,216 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" s="13" t="s">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="13" t="s">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="13" t="s">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" s="13" t="s">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="13" t="s">
+    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="13" t="s">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="B16" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Use percent instead of counts for CorrectedGermSpeed
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200D58D-259B-41E5-93E1-4C1259BFC8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB9E286-35D5-4240-9152-E27ED88F0B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="203">
   <si>
     <t>Germination index</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>Time required for $x$\% of total seeds to germinate.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Peak value($PV$) (Czabator) or Emergence Energy ($EE$)</t>
@@ -560,11 +557,6 @@
     <t>With argument `method` specified as `"farooq"`, it is computed as follows.
 $$t_{50}=T_{i}+\frac{(\frac{N}{2}-N_{i})(T_{j}-T_{i})}{N_{j}-N_{i}}$$
 Where, $t_{50}$ is the median germination time, $N$ is the final number of germinated seeds, and $N_{i}$ and $N_{j}$ are the total number of seeds germinated in adjacent counts at time $T_{i}$ and $T_{j}$ respectively, when $N_{i} &lt; \frac{N}{2} &lt; N_{j}$.</t>
-  </si>
-  <si>
-    <t>It is computed as follows.
-$$S_{corrected} = \frac{S}{FGP}$$
-Where, $FGP$ is the final germination percentage or germinability.</t>
   </si>
   <si>
     <t>It is estimated as follows.
@@ -729,6 +721,11 @@
   </si>
   <si>
     <t>\%^2^ time^-1^</t>
+  </si>
+  <si>
+    <t>It is computed as follows.
+$$S_{corrected} = \frac{S}{FGP}$$
+Where, $S$ is the germination speed computed with germination percentage instead of counts and $FGP$ is the final germination percentage or germinability.</t>
   </si>
 </sst>
 </file>
@@ -1184,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1200,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1220,13 +1217,13 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>112</v>
@@ -1240,13 +1237,13 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>112</v>
@@ -1255,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1266,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1286,7 +1283,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -1320,13 +1317,13 @@
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>8</v>
@@ -1346,7 +1343,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>8</v>
@@ -1366,7 +1363,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
@@ -1380,13 +1377,13 @@
     </row>
     <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -1395,7 +1392,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1406,7 +1403,7 @@
         <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>58</v>
@@ -1426,7 +1423,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>8</v>
@@ -1446,7 +1443,7 @@
         <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>58</v>
@@ -1466,7 +1463,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>113</v>
@@ -1475,7 +1472,7 @@
         <v>18</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1506,7 +1503,7 @@
         <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>58</v>
@@ -1540,22 +1537,22 @@
     </row>
     <row r="18" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="135" x14ac:dyDescent="0.25">
@@ -1566,10 +1563,10 @@
         <v>32</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>62</v>
@@ -1578,7 +1575,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>58</v>
@@ -1606,7 +1603,7 @@
         <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>112</v>
@@ -1626,7 +1623,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>113</v>
@@ -1646,10 +1643,10 @@
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>62</v>
@@ -1666,7 +1663,7 @@
         <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>112</v>
@@ -1675,21 +1672,21 @@
         <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>62</v>
@@ -1700,13 +1697,13 @@
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>113</v>
@@ -1720,16 +1717,16 @@
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>62</v>
@@ -1740,13 +1737,13 @@
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>8</v>
@@ -1755,18 +1752,18 @@
         <v>62</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>8</v>
@@ -1775,98 +1772,98 @@
         <v>62</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>113</v>
@@ -1880,22 +1877,22 @@
     </row>
     <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>62</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="165" x14ac:dyDescent="0.25">
@@ -1906,10 +1903,10 @@
         <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>62</v>
@@ -1926,16 +1923,16 @@
         <v>30</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>59</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -1946,16 +1943,16 @@
         <v>96</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1966,7 +1963,7 @@
         <v>41</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>73</v>
@@ -1986,10 +1983,10 @@
         <v>40</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>68</v>
@@ -2087,7 +2084,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>8</v>
@@ -2185,7 +2182,7 @@
         <v>91</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>8</v>
@@ -2225,7 +2222,7 @@
         <v>78</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>

</xml_diff>

<commit_message>
Fix bib refrence key lyon_rapid_1966
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31CDB5B-17EC-46BA-89E9-0770D17E33E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4382950B-93B1-41E4-A3B4-61BAA63E3292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,10 +722,10 @@
     <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbach_tillage_1982; @aosa_seed_1983; @khandakar_jute_1983; @hsu_planting_1986; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
   </si>
   <si>
-    <t>[@grose_laboratory_1958; @timson_new_1965; @lyonRapidMethodDetermining1966; @chaudhary_effect_1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
-  </si>
-  <si>
     <t>[@george_influence_1961; @tucker_estimating_1965; @nichols_two_1968;@chopra_effect_1980]</t>
+  </si>
+  <si>
+    <t>[@grose_laboratory_1958; @timson_new_1965; @lyon_rapid_1966; @chaudhary_effect_1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
   </si>
 </sst>
 </file>
@@ -1136,7 +1136,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1626,7 @@
         <v>62</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>62</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added abbr for Speed of germination
</commit_message>
<xml_diff>
--- a/vignettes/Indices.xlsx
+++ b/vignettes/Indices.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4382950B-93B1-41E4-A3B4-61BAA63E3292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B4EC25-4F9E-4A77-A0DD-5319CDD6D0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,12 +79,6 @@
     <t>Germination rate</t>
   </si>
   <si>
-    <t>Speed of accumulated germination</t>
-  </si>
-  <si>
-    <t>Corrected germination rate index</t>
-  </si>
-  <si>
     <t>[@edwards_temperature_1932]</t>
   </si>
   <si>
@@ -414,9 +408,6 @@
   </si>
   <si>
     <t>Mean germination time or Mean length of incubation time ($\overline{T}$) or Germination resistance ($GR$) or Sprouting index ($SI$) or Emergence index ($EI$)</t>
-  </si>
-  <si>
-    <t>Speed of germination or Germination rate Index or index of velocity of germination or Emergence rate index (Allan, Vogel and Peterson; Erbach; Hsu and Nelson) or Germination index (AOSA)</t>
   </si>
   <si>
     <t>Function</t>
@@ -693,39 +684,51 @@
     <t>\%^2^ time^-1^</t>
   </si>
   <si>
+    <t>[@shmueli_emergence_1971]</t>
+  </si>
+  <si>
+    <t>[@shmueli_emergence_1971; @de_santana_alise_2004; @ranal_how_2006]</t>
+  </si>
+  <si>
+    <t>[@bilbro_soil_1982]</t>
+  </si>
+  <si>
+    <t>[@fakorede_relation_1980; @fakorede_variability_1981; @fakorede_heterotic_1983]</t>
+  </si>
+  <si>
+    <t>[@melville_seed_1980]</t>
+  </si>
+  <si>
+    <t>[@melville_seed_1980; @de_santana_alise_2004; @ranal_how_2006]</t>
+  </si>
+  <si>
+    <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @mock_cold_1972; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
+  </si>
+  <si>
+    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbach_tillage_1982; @aosa_seed_1983; @khandakar_jute_1983; @hsu_planting_1986; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
+  </si>
+  <si>
+    <t>[@george_influence_1961; @tucker_estimating_1965; @nichols_two_1968;@chopra_effect_1980]</t>
+  </si>
+  <si>
+    <t>[@grose_laboratory_1958; @timson_new_1965; @lyon_rapid_1966; @chaudhary_effect_1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
+  </si>
+  <si>
+    <t>Speed of germination ($S$) or Germination rate Index or index of velocity of germination or Emergence rate index (Allan, Vogel and Peterson; Erbach; Hsu and Nelson) or Germination index (AOSA)</t>
+  </si>
+  <si>
+    <t>Speed of accumulated germination ($S_{accumulated}$)</t>
+  </si>
+  <si>
+    <t>Corrected speed of germination or Corrected germination rate index ($\hat{S}$)</t>
+  </si>
+  <si>
     <t>It is computed as follows.
 $$S_{corrected} = \frac{S}{FGP}$$
-Where, $S$ is the germination speed computed with germination percentage instead of counts and $FGP$ is the final germination percentage or germinability.</t>
-  </si>
-  <si>
-    <t>[@shmueli_emergence_1971]</t>
-  </si>
-  <si>
-    <t>[@shmueli_emergence_1971; @de_santana_alise_2004; @ranal_how_2006]</t>
-  </si>
-  <si>
-    <t>[@bilbro_soil_1982]</t>
-  </si>
-  <si>
-    <t>[@fakorede_relation_1980; @fakorede_variability_1981; @fakorede_heterotic_1983]</t>
-  </si>
-  <si>
-    <t>[@melville_seed_1980]</t>
-  </si>
-  <si>
-    <t>[@melville_seed_1980; @de_santana_alise_2004; @ranal_how_2006]</t>
-  </si>
-  <si>
-    <t>[@edmond_effects_1958; @czabator_germination_1962; @smith_germinating_1964; @gordon_observations_1969; @gordon_germination_1971; @mock_cold_1972; @ellis_improved_1980 @labouriau_germinacao_1983; @ranal_how_2006]</t>
-  </si>
-  <si>
-    <t>[@throneberry_relation_1955; @maguire_speed_1962; @allan_seedling_1962; @kendrick_photocontrol_1969; @bouton_germination_1976; @erbach_tillage_1982; @aosa_seed_1983; @khandakar_jute_1983; @hsu_planting_1986; @bradbeer_seed_1988; @wardle_allelopathic_1991]</t>
-  </si>
-  <si>
-    <t>[@george_influence_1961; @tucker_estimating_1965; @nichols_two_1968;@chopra_effect_1980]</t>
-  </si>
-  <si>
-    <t>[@grose_laboratory_1958; @timson_new_1965; @lyon_rapid_1966; @chaudhary_effect_1970; @negm_effects_1978; @brown_representing_1988; @baskin_seeds_1998; @goodchild_method_1971]</t>
+Where, $S$ is the germination speed computed with germination percentage instead of counts and $FGP$ is the final germination percentage or germinability.
+It can also be computed from speed of accumulated germination (computed with germination percentage).
+$$\hat{S}_{accumulated} = \frac{S_{accumulated}}{FGP}$$
+Where, $S_{accumulated}$ is the speed of accumulated germination computed with germination percentage instead of counts and $FGP$ is the final germination percentage or germinability.</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -1171,42 +1174,42 @@
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1217,7 +1220,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
@@ -1226,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -1237,7 +1240,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>8</v>
@@ -1246,18 +1249,18 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -1266,18 +1269,18 @@
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>8</v>
@@ -1286,18 +1289,18 @@
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>8</v>
@@ -1311,13 +1314,13 @@
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
@@ -1331,13 +1334,13 @@
     </row>
     <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>8</v>
@@ -1346,38 +1349,38 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>8</v>
@@ -1386,567 +1389,567 @@
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>200</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>186</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1971,7 +1974,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -1985,23 +1988,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -2009,10 +2012,10 @@
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
@@ -2021,10 +2024,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>8</v>
@@ -2035,10 +2038,10 @@
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>8</v>
@@ -2049,10 +2052,10 @@
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>8</v>
@@ -2063,10 +2066,10 @@
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>8</v>
@@ -2077,10 +2080,10 @@
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>8</v>
@@ -2091,10 +2094,10 @@
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>8</v>
@@ -2105,10 +2108,10 @@
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>8</v>
@@ -2119,10 +2122,10 @@
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -2133,10 +2136,10 @@
     </row>
     <row r="13" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -2147,22 +2150,22 @@
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>91</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>8</v>
@@ -2173,10 +2176,10 @@
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>

</xml_diff>